<commit_message>
Initial commit v1p3, R2019a
</commit_message>
<xml_diff>
--- a/SimResults/sm_car_results.xlsx
+++ b/SimResults/sm_car_results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\simscape\demos\allsimscape\cars\vehicle-templates\SimResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC8BD6D-510C-4C87-A686-06350C6BEBDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A00673-F30F-4DB1-9380-A60F8B1A350E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="4644" windowWidth="15264" windowHeight="7356" xr2:uid="{040A6F09-DF37-4201-87A6-29EA35F967C7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" xr2:uid="{A0ED6085-80D8-4D2A-8B80-6ABD2C7BE595}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="130" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,12 +32,27 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,14 +72,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{2C5E4C91-330C-4989-A6F1-B4C16FA6AA07}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{4C0561CC-46A1-4576-BB39-5A5447F23952}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,10 +394,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46DF5C8-ADC5-4E3A-A39D-A7372ACE16C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF14B61A-6309-4E02-BAE5-C28962867430}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Initial commit v1p5, R2020b.
</commit_message>
<xml_diff>
--- a/SimResults/sm_car_results.xlsx
+++ b/SimResults/sm_car_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\simscape\demos\allsimscape\cars\vehicle-templates\SimResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\vehicle-templates\SimResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD92C1CD-B08D-4EF3-8117-FCC70335FDAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1917D8AF-2ABA-412B-85D1-7A25224810F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2904" windowWidth="14400" windowHeight="7908" xr2:uid="{86C44CE1-1010-4E30-92B1-BDE677C7682C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{86C44CE1-1010-4E30-92B1-BDE677C7682C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>

</xml_diff>